<commit_message>
updated dataset with imputation
</commit_message>
<xml_diff>
--- a/Data/Terridata/fisc_new.xlsx
+++ b/Data/Terridata/fisc_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hertieschool-my.sharepoint.com/personal/226679_students_hertie-school_org/Documents/GitHub/MDS_thesis/Data/Terridata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4FE656B6-EA56-44A2-B845-8F0EFF729537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B95DC4DB-EECD-4F96-BE96-6700AD1FCA2D}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{4FE656B6-EA56-44A2-B845-8F0EFF729537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B0A146-398E-4D3B-8313-96A93BDC69D5}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{FF7FDEB9-8933-4A47-8676-4D15A1FE4831}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF7FDEB9-8933-4A47-8676-4D15A1FE4831}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3913,7 +3913,7 @@
   <dimension ref="A1:C3305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>